<commit_message>
reorganization and selection data
</commit_message>
<xml_diff>
--- a/experimental_data_collection/fitness_selection/fitness_selection_validation.xlsx
+++ b/experimental_data_collection/fitness_selection/fitness_selection_validation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/REU/REU-Drone-Swarm-Optimization/experimental_data_collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/REU/REU-Drone-Swarm-Optimization/experimental_data_collection/fitness_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{799A8E10-B3F9-854D-9488-0845D5530158}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982BB32E-8201-694D-AD02-3120584F25B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{87A588F9-9300-0449-838A-6A4B9E2E6CA4}"/>
   </bookViews>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>runtime</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t># of UAVs</t>
-  </si>
-  <si>
-    <t>user cover</t>
-  </si>
-  <si>
-    <t>trial</t>
   </si>
   <si>
     <t>Fitness Function Experimental Data</t>
@@ -52,6 +43,27 @@
   </si>
   <si>
     <t>Users Provided Coverage</t>
+  </si>
+  <si>
+    <t>Natural Selection Experimental Data</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>User Cover</t>
+  </si>
+  <si>
+    <t>Combining Coordinates</t>
+  </si>
+  <si>
+    <t>Averging Coordinates</t>
+  </si>
+  <si>
+    <t>*user coverage must be 100% by def of selected fitness function</t>
+  </si>
+  <si>
+    <t>Runtime (s)</t>
   </si>
 </sst>
 </file>
@@ -92,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -229,11 +241,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -252,6 +273,11 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,14 +287,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1535,6 +1569,829 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runtime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Proposed Algorithm with Different Natural Selection Methods</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$B$23,Sheet1!$B$28)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Combining Coordinates</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Averging Coordinates</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$C$27,Sheet1!$C$32)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>34.300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>511</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E277-FA41-B04C-AF12D93CB9F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="529348959"/>
+        <c:axId val="529327775"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="529348959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Natural</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Selection Method</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529327775"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="529327775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Rumtimr (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529348959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of UAVs used by Proposed Algorithm with Different Natural Selection Methods</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$B$23,Sheet1!$B$28)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Combining Coordinates</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Averging Coordinates</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$D$27,Sheet1!$D$32)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.666666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BB6C-CF4B-8260-3C751DD4F5CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="532296383"/>
+        <c:axId val="532075615"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="532296383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Natural Selection</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Method</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532075615"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="532075615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of UAVs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532296383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1655,6 +2512,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3164,18 +4101,1024 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -3204,16 +5147,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3240,16 +5183,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3269,6 +5212,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{773610E9-6EDE-864F-8132-D7D049CFA609}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82DADD57-8C92-AA41-BEAF-F3BE8DFC3330}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3574,10 +5589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3562F8F-FEE0-E442-857D-A24E541763BC}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3594,46 +5609,46 @@
       <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="B2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
-      <c r="B4" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -3694,13 +5709,13 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <f>AVERAGE(C5:C7)</f>
         <v>49.733333333333327</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="19">
         <f>AVERAGE(D5:D7)</f>
         <v>1</v>
       </c>
@@ -3710,12 +5725,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
@@ -3738,7 +5753,7 @@
       <c r="C11" s="3">
         <v>188</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="20">
         <v>0.67500000000000004</v>
       </c>
       <c r="E11" s="10">
@@ -3761,13 +5776,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1">
         <f>AVERAGE(C10:C12)</f>
         <v>163</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="22">
         <f>AVERAGE(D10:D12)</f>
         <v>0.62500000000000011</v>
       </c>
@@ -3777,12 +5792,12 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
@@ -3819,7 +5834,7 @@
       <c r="C17" s="6">
         <v>241</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="21">
         <v>0.72499999999999998</v>
       </c>
       <c r="E17" s="6">
@@ -3828,13 +5843,13 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1">
         <f>AVERAGE(C15:C17)</f>
         <v>242.96666666666667</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="22">
         <f>AVERAGE(D15:D17)</f>
         <v>0.69166666666666676</v>
       </c>
@@ -3843,12 +5858,152 @@
         <v>10</v>
       </c>
     </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>31.8</v>
+      </c>
+      <c r="D24" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D25" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="4">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4">
+        <v>34.9</v>
+      </c>
+      <c r="D26" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <f>AVERAGE(C24:C26)</f>
+        <v>34.300000000000004</v>
+      </c>
+      <c r="D27" s="1">
+        <f>AVERAGE(D24:D26)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>447</v>
+      </c>
+      <c r="D29" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>535</v>
+      </c>
+      <c r="D30" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="4">
+        <v>3</v>
+      </c>
+      <c r="C31" s="4">
+        <v>551</v>
+      </c>
+      <c r="D31" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1">
+        <f>AVERAGE(C29:C31)</f>
+        <v>511</v>
+      </c>
+      <c r="D32" s="1">
+        <f>AVERAGE(D29:D31)</f>
+        <v>13.666666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B33:D34"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>